<commit_message>
20250203 add gimmick info
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/GimmickDB.xlsx
+++ b/casual1/Assets/Resources/GimmickDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,10 +141,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>해당 영역을 통과해서 히트 시, 데미지가 N배(1차 구현 완)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>히트 시 회전속도 증가(1차 구현 완)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -170,6 +166,86 @@
   </si>
   <si>
     <t>Undo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 영역을 통과해서 히트 시, 데미지없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 영역을 통과해서 히트 시, 데미지 추가1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>color</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bomb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnOff(ON)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnOff(Off)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedUp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpeedDown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddShot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Damage Area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No Damage Area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chain Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iron Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target Heart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gimmick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>textinfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>textinfo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,7 +253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +283,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,10 +312,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -512,22 +598,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="56.625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-    <col min="7" max="7" width="16.75" customWidth="1"/>
-    <col min="8" max="9" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="10.625" customWidth="1"/>
+    <col min="8" max="8" width="16.75" customWidth="1"/>
+    <col min="9" max="10" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,28 +622,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10100</v>
       </c>
@@ -566,325 +662,411 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>0.4</v>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10200</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>0.4</v>
-      </c>
       <c r="E3">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G3">
+        <v>0.4</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10300</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>0.4</v>
-      </c>
       <c r="E4">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G4">
+        <v>0.4</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10400</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5">
-        <v>0.4</v>
-      </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F5">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G5">
+        <v>0.4</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10500</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
-        <v>0.4</v>
-      </c>
       <c r="E6">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G6">
+        <v>0.4</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10600</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7">
-        <v>0.4</v>
-      </c>
       <c r="E7">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F7">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G7">
+        <v>0.4</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10700</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>0.4</v>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
       </c>
       <c r="E8">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G8">
+        <v>0.4</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10800</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>0.4</v>
+      <c r="C9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
       </c>
       <c r="E9">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10900</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="D10">
-        <v>0.4</v>
-      </c>
       <c r="E10">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F10">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G10">
+        <v>0.4</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11000</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="D11">
-        <v>0.4</v>
-      </c>
       <c r="E11">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G11">
+        <v>0.4</v>
+      </c>
+      <c r="H11">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12">
-        <v>0.4</v>
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
       </c>
       <c r="E12">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G12">
+        <v>0.4</v>
+      </c>
+      <c r="H12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20200</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13">
-        <v>0.4</v>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
       </c>
       <c r="E13">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G13">
+        <v>0.4</v>
+      </c>
+      <c r="H13">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20300</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="D14">
-        <v>0.4</v>
-      </c>
       <c r="E14">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F14">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G14">
+        <v>0.4</v>
+      </c>
+      <c r="H14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>30100</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15">
-        <v>0.4</v>
-      </c>
-      <c r="E15">
-        <v>0.8</v>
-      </c>
-      <c r="F15">
-        <v>0.4</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
+        <v>38</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>30200</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>